<commit_message>
Add game modes to capture speed graph
</commit_message>
<xml_diff>
--- a/tips_and_tricks/files/squad_capture_speed.xlsx
+++ b/tips_and_tricks/files/squad_capture_speed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexey\Desktop\squad\squad_guides\tips_and_tricks\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302B6354-43BC-4DC3-944B-38F1017E4E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAFF472-488D-41A5-8861-BC37F269E0C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A523BE98-B88B-4CE6-941F-24AA777ACBB6}"/>
   </bookViews>
@@ -30,12 +30,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Team Count</t>
   </si>
   <si>
-    <t>Capture Speed AAS/RAAS/Invasion v.8.1</t>
+    <t>Skirmish v2.15</t>
+  </si>
+  <si>
+    <t>TC v2.15</t>
+  </si>
+  <si>
+    <t>Capture Speed AAS/RAAS/Invasion v8.1</t>
   </si>
 </sst>
 </file>
@@ -141,7 +147,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.31503889576681238"/>
-          <c:y val="4.208234720090262E-2"/>
+          <c:y val="1.8680478631326679E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -180,10 +186,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.6872131341967446E-2"/>
-          <c:y val="0.15866977810950297"/>
-          <c:w val="0.89019685039370078"/>
-          <c:h val="0.70236913094196562"/>
+          <c:x val="8.5128819106372655E-2"/>
+          <c:y val="0.11980851823998681"/>
+          <c:w val="0.90240004678116614"/>
+          <c:h val="0.51433165020599769"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -198,7 +204,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Capture Speed AAS/RAAS/Invasion v.8.1</c:v>
+                  <c:v>Capture Speed AAS/RAAS/Invasion v8.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -232,8 +238,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.6921270784022434E-2"/>
-                  <c:y val="-8.0983942712781629E-2"/>
+                  <c:x val="-2.6921270784022421E-2"/>
+                  <c:y val="-6.8291829795101539E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -565,7 +571,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -651,6 +657,278 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F967-48E0-BF2B-3464B7D35BE0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Skirmish v2.15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D663-47D1-B651-37EFAD485110}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TC v2.15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="uk-UA"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D663-47D1-B651-37EFAD485110}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -736,8 +1014,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.25433456742452248"/>
-              <c:y val="0.94356354089263739"/>
+              <c:x val="0.25956450413130683"/>
+              <c:y val="0.6888958568084208"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -858,8 +1136,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="6.0244478264396776E-3"/>
-              <c:y val="0.15152516753551251"/>
+              <c:x val="1.6484321240008381E-2"/>
+              <c:y val="5.5653134189637896E-3"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -939,15 +1217,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.27584086332116353"/>
-          <c:y val="0.22191452037031362"/>
-          <c:w val="0.45851157099474366"/>
-          <c:h val="5.7355698830668531E-2"/>
+          <c:x val="8.0357085253321803E-2"/>
+          <c:y val="0.77942520493595202"/>
+          <c:w val="0.33737662805802016"/>
+          <c:h val="0.22057479506404795"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1570,15 +1848,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>197068</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>155684</xdr:rowOff>
+      <xdr:colOff>183930</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>11167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>151085</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>157655</xdr:rowOff>
+      <xdr:colOff>137947</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>13137</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1610,12 +1888,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.76844</cdr:x>
-      <cdr:y>0.11523</cdr:y>
+      <cdr:x>0.7367</cdr:x>
+      <cdr:y>0.79072</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.97115</cdr:x>
-      <cdr:y>0.29444</cdr:y>
+      <cdr:x>0.95444</cdr:x>
+      <cdr:y>0.96184</cdr:y>
     </cdr:to>
     <cdr:pic>
       <cdr:nvPicPr>
@@ -1643,8 +1921,8 @@
       </cdr:blipFill>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5598069" y="417302"/>
-          <a:ext cx="1476707" cy="648998"/>
+          <a:off x="5366846" y="3164823"/>
+          <a:ext cx="1586208" cy="684900"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1952,107 +2230,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE16B79-BECE-4E8B-8277-6A92E1AB559C}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>220</v>
       </c>
       <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
       <c r="B3">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>52</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>180</v>
       </c>
       <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>165</v>
       </c>
       <c r="B5">
+        <v>82</v>
+      </c>
+      <c r="C5">
+        <v>41</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>150</v>
       </c>
       <c r="B6">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>37.6</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>135</v>
       </c>
       <c r="B7">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>120</v>
       </c>
       <c r="B8">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>100</v>
       </c>
       <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>77</v>
       </c>
-      <c r="B10">
+      <c r="D10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>47</v>
       </c>
-      <c r="B11">
+      <c r="D11">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upd graph with neutral aas number bonus
</commit_message>
<xml_diff>
--- a/tips_and_tricks/files/squad_capture_speed.xlsx
+++ b/tips_and_tricks/files/squad_capture_speed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexey\Desktop\squad\squad_guides\tips_and_tricks\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAFF472-488D-41A5-8861-BC37F269E0C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD3B17D-557E-4047-AB95-63EDEA3CF35B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A523BE98-B88B-4CE6-941F-24AA777ACBB6}"/>
   </bookViews>
@@ -214,6 +214,7 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -233,6 +234,108 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-781C-4A1D-A7BB-2BFDFB36E67A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-781C-4A1D-A7BB-2BFDFB36E67A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-781C-4A1D-A7BB-2BFDFB36E67A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -2233,7 +2336,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>